<commit_message>
UML aanvulling + correctie connectxinterface
</commit_message>
<xml_diff>
--- a/docs/UML.xlsx
+++ b/docs/UML.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\1e Bachelor TI\S2\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Documents\1e Bachelor TI\S2\Project\GitHub\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Chronologisch" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>ConnectX</t>
   </si>
@@ -127,13 +127,70 @@
   </si>
   <si>
     <t>ConnectXInterface</t>
+  </si>
+  <si>
+    <t>scorePlayer1: int</t>
+  </si>
+  <si>
+    <t>scorePlayer2: int</t>
+  </si>
+  <si>
+    <t>playerAtPlay: int</t>
+  </si>
+  <si>
+    <t>namePlayer1: string</t>
+  </si>
+  <si>
+    <t>namePlayer2: string</t>
+  </si>
+  <si>
+    <t>game: ConnectX</t>
+  </si>
+  <si>
+    <t>ConnectXInterface()</t>
+  </si>
+  <si>
+    <t>newGame(): public void</t>
+  </si>
+  <si>
+    <t>newGame(int players, int rows, int columns): public void</t>
+  </si>
+  <si>
+    <t>newGame(int players, int rows, int columns, int tokenStreak): public void</t>
+  </si>
+  <si>
+    <t>gameRunning(): public bool</t>
+  </si>
+  <si>
+    <t>setScorePlayer(int player): public void</t>
+  </si>
+  <si>
+    <t>getScore(int player): public int</t>
+  </si>
+  <si>
+    <t>setPlayerAtPlay(int playerAtPlay): public void</t>
+  </si>
+  <si>
+    <t>getplayerAtPlay(): public int</t>
+  </si>
+  <si>
+    <t>switchPlayerAtPlay(): public void</t>
+  </si>
+  <si>
+    <t>isCurrentGameWon(): public bool</t>
+  </si>
+  <si>
+    <t>reset(): public void</t>
+  </si>
+  <si>
+    <t xml:space="preserve">getToken(int row, int column): </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +206,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -158,7 +223,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -166,13 +231,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -453,21 +529,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,162 +551,399 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
       <c r="B27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
       <c r="B28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
       <c r="B29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
       <c r="B30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
       <c r="B32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -645,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>

</xml_diff>

<commit_message>
rearranged tests + edit UML
</commit_message>
<xml_diff>
--- a/docs/UML.xlsx
+++ b/docs/UML.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="171">
   <si>
     <t>raster: int[,]</t>
   </si>
@@ -496,9 +496,6 @@
   </si>
   <si>
     <t>TestNewGameWith10RowsAnd14Columns(): public void</t>
-  </si>
-  <si>
-    <t>TestResetGame(): public void</t>
   </si>
   <si>
     <t>TestCurrentGameWon(): public void</t>
@@ -883,9 +880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,10 +914,10 @@
         <v>96</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1052,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1096,7 +1093,7 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1140,7 +1137,7 @@
         <v>5</v>
       </c>
       <c r="N6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1184,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="N7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1225,7 +1222,7 @@
         <v>7</v>
       </c>
       <c r="N8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1266,7 +1263,7 @@
         <v>8</v>
       </c>
       <c r="N9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1307,7 +1304,7 @@
         <v>9</v>
       </c>
       <c r="N10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1348,7 +1345,7 @@
         <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1389,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="N12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1489,12 +1486,6 @@
       </c>
       <c r="J15" t="s">
         <v>127</v>
-      </c>
-      <c r="K15">
-        <v>14</v>
-      </c>
-      <c r="L15" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>